<commit_message>
PyCharm Commit - Commit before rewriting AI
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicola_BLJv2\Desktop\SSPAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6523FA86-3D97-41A7-81BE-D171BA551619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3E742A-90AA-4D53-9DFD-5E5BD56D27D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-1050" windowWidth="19394" windowHeight="10395" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1726,7 +1726,7 @@
                   <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.25</c:v>
+                  <c:v>51.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2233,8 +2233,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AU27" sqref="AU27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AM26" sqref="AM26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>44.25</v>
+        <v>51.25</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3664,7 +3664,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>15.75</v>
+        <v>20.75</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3707,7 +3707,9 @@
       <c r="AI20" s="59"/>
       <c r="AJ20" s="60"/>
       <c r="AK20" s="55"/>
-      <c r="AL20" s="55"/>
+      <c r="AL20" s="55">
+        <v>5</v>
+      </c>
       <c r="AM20" s="56"/>
       <c r="AN20" s="57"/>
       <c r="AO20" s="58"/>
@@ -3899,7 +3901,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="51"/>
@@ -3938,7 +3940,9 @@
       <c r="AK23" s="63">
         <v>8</v>
       </c>
-      <c r="AL23" s="63"/>
+      <c r="AL23" s="63">
+        <v>2</v>
+      </c>
       <c r="AM23" s="63"/>
       <c r="AN23" s="57"/>
       <c r="AO23" s="58"/>
@@ -5333,7 +5337,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>49.4</v>
+        <v>56.4</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5463,7 +5467,7 @@
       </c>
       <c r="AL43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AM43" s="39">
         <f t="shared" ref="AM43:BD43" si="4">SUM(AM9:AM42)</f>
@@ -5665,7 +5669,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>44.25</v>
+        <v>51.25</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
PyCharm Commit - Commit with first AI [AI Not Working Yet]
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicola_BLJv2\Desktop\SSPAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3E742A-90AA-4D53-9DFD-5E5BD56D27D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67C7E3F-AB8C-4A60-A59A-987497680537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-1050" windowWidth="19394" windowHeight="10395" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1720,13 +1720,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.4</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.25</c:v>
+                  <c:v>71.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1735,7 +1735,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2233,8 +2233,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AM26" sqref="AM26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AZ41" sqref="AZ41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -3065,7 +3065,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -3107,7 +3107,9 @@
       <c r="AJ12" s="60"/>
       <c r="AK12" s="61"/>
       <c r="AL12" s="61"/>
-      <c r="AM12" s="63"/>
+      <c r="AM12" s="63">
+        <v>0.5</v>
+      </c>
       <c r="AN12" s="57"/>
       <c r="AO12" s="58"/>
       <c r="AP12" s="59"/>
@@ -3518,7 +3520,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>51.25</v>
+        <v>71.25</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3901,7 +3903,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="51"/>
@@ -3943,13 +3945,19 @@
       <c r="AL23" s="63">
         <v>2</v>
       </c>
-      <c r="AM23" s="63"/>
+      <c r="AM23" s="63">
+        <v>7</v>
+      </c>
       <c r="AN23" s="57"/>
       <c r="AO23" s="58"/>
       <c r="AP23" s="59"/>
       <c r="AQ23" s="60"/>
-      <c r="AR23" s="63"/>
-      <c r="AS23" s="63"/>
+      <c r="AR23" s="63">
+        <v>8</v>
+      </c>
+      <c r="AS23" s="63">
+        <v>5</v>
+      </c>
       <c r="AT23" s="63"/>
       <c r="AU23" s="57"/>
       <c r="AV23" s="58"/>
@@ -5054,7 +5062,7 @@
       </c>
       <c r="D39" s="42">
         <f>SUM(D40:D42)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E39" s="32"/>
       <c r="F39" s="31"/>
@@ -5125,7 +5133,7 @@
       <c r="C40" s="49"/>
       <c r="D40" s="83">
         <f>SUM(G40:BJ40)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E40" s="50"/>
       <c r="F40" s="51"/>
@@ -5167,7 +5175,9 @@
       <c r="AP40" s="53"/>
       <c r="AQ40" s="54"/>
       <c r="AR40" s="55"/>
-      <c r="AS40" s="55"/>
+      <c r="AS40" s="55">
+        <v>3</v>
+      </c>
       <c r="AT40" s="56"/>
       <c r="AU40" s="57"/>
       <c r="AV40" s="58"/>
@@ -5337,7 +5347,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>56.4</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5471,7 +5481,7 @@
       </c>
       <c r="AM43" s="39">
         <f t="shared" ref="AM43:BD43" si="4">SUM(AM9:AM42)</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="AN43" s="39">
         <f t="shared" si="4"/>
@@ -5491,11 +5501,11 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AT43" s="39">
         <f t="shared" si="4"/>
@@ -5635,7 +5645,7 @@
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
@@ -5669,7 +5679,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>51.25</v>
+        <v>71.25</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
@@ -5718,7 +5728,7 @@
       </c>
       <c r="D8" s="80">
         <f>Zeitplanung!D39</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="81"/>
     </row>

</xml_diff>